<commit_message>
Can pause during combat
global.turn=0 means the game is paused
added some sprites and animation
all rooms based on position
</commit_message>
<xml_diff>
--- a/Project1.gmx/Generals and Soldiers.xlsx
+++ b/Project1.gmx/Generals and Soldiers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>Variable</t>
   </si>
@@ -171,19 +171,16 @@
     <t>alternate spawn patterns</t>
   </si>
   <si>
-    <t>animate enemy movement</t>
-  </si>
-  <si>
-    <t>enemy color?</t>
-  </si>
-  <si>
     <t>change direction</t>
   </si>
   <si>
-    <t>enemy general board</t>
-  </si>
-  <si>
-    <t>track score with board</t>
+    <t>enemy sprites</t>
+  </si>
+  <si>
+    <t>game name on pause menu</t>
+  </si>
+  <si>
+    <t>align lesser congratulatory message</t>
   </si>
 </sst>
 </file>
@@ -902,10 +899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -925,12 +922,12 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -941,11 +938,6 @@
     <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checks for attacks all 4 directions
</commit_message>
<xml_diff>
--- a/Project1.gmx/Generals and Soldiers.xlsx
+++ b/Project1.gmx/Generals and Soldiers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>Variable</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>turns</t>
+  </si>
+  <si>
+    <t>sprite animation script</t>
+  </si>
+  <si>
+    <t>spawn scripts</t>
+  </si>
+  <si>
+    <t>set board space to noone when dead</t>
   </si>
 </sst>
 </file>
@@ -899,10 +908,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -938,6 +947,21 @@
     <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>